<commit_message>
added few more missing genres
</commit_message>
<xml_diff>
--- a/data/hollywoodStories_consol.xlsx
+++ b/data/hollywoodStories_consol.xlsx
@@ -7561,10 +7561,10 @@
   <dimension ref="A1:U998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N876" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H49" sqref="H49"/>
+      <selection pane="bottomRight" activeCell="U901" sqref="U901"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -37427,7 +37427,10 @@
         <v>201</v>
       </c>
       <c r="E452">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="F452">
+        <v>87</v>
       </c>
       <c r="H452" t="s">
         <v>25</v>
@@ -37465,7 +37468,7 @@
       </c>
       <c r="U452">
         <f>Table1[[#This Row],[scoreAudience]]-Table1[[#This Row],[scoreRotten]]</f>
-        <v>-74</v>
+        <v>12</v>
       </c>
     </row>
     <row r="453" spans="1:21" x14ac:dyDescent="0.45">
@@ -61797,7 +61800,7 @@
         <v>92</v>
       </c>
       <c r="H822" t="s">
-        <v>883</v>
+        <v>94</v>
       </c>
       <c r="I822">
         <v>666</v>
@@ -63260,16 +63263,16 @@
         <v>1290</v>
       </c>
       <c r="E845">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F845">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G845" t="s">
         <v>131</v>
       </c>
       <c r="H845" t="s">
-        <v>94</v>
+        <v>375</v>
       </c>
       <c r="I845">
         <v>2874</v>
@@ -63310,7 +63313,7 @@
       </c>
       <c r="U845">
         <f>Table1[[#This Row],[scoreAudience]]-Table1[[#This Row],[scoreRotten]]</f>
-        <v>-41</v>
+        <v>-37</v>
       </c>
     </row>
     <row r="846" spans="1:21" x14ac:dyDescent="0.45">
@@ -66659,7 +66662,7 @@
         <v>9729.5534591194973</v>
       </c>
       <c r="T904">
-        <v>5313987.22</v>
+        <v>287334279</v>
       </c>
       <c r="U904">
         <f>Table1[[#This Row],[scoreAudience]]-Table1[[#This Row],[scoreRotten]]</f>

</xml_diff>